<commit_message>
Add time estimations and pricing.
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Task name</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Discussions and meetings (emails, skypes)</t>
   </si>
   <si>
-    <t>Time spent during meetings, discussion, oral chat and so on.</t>
-  </si>
-  <si>
     <t>2h for the moment</t>
   </si>
   <si>
@@ -166,6 +163,15 @@
   </si>
   <si>
     <t>Responsable</t>
+  </si>
+  <si>
+    <t>Test: Generate a YAML file</t>
+  </si>
+  <si>
+    <t>Test: Generate the Ansible command</t>
+  </si>
+  <si>
+    <t>Time spent during oral meetings, discussion, emails and so on.</t>
   </si>
 </sst>
 </file>
@@ -593,7 +599,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -661,6 +667,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="2">
+        <f>B3*30</f>
         <v>90</v>
       </c>
     </row>
@@ -678,6 +685,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="2">
+        <f t="shared" ref="F4:F19" si="0">B4*30</f>
         <v>45</v>
       </c>
     </row>
@@ -692,6 +700,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
@@ -703,30 +712,120 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="8">
         <f>SUM(B3:B19)</f>
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10">
         <f>SUM(F2:F19)</f>
-        <v>825</v>
+        <v>885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add YAML writer. Works correctly. Add unit tests with mocha. Updated task list.
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -156,9 +156,6 @@
     <t>2h for the moment</t>
   </si>
   <si>
-    <t>Total:</t>
-  </si>
-  <si>
     <t>Estimated time (h)</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>Time spent during oral meetings, discussion, emails and so on.</t>
+  </si>
+  <si>
+    <t>Total: (Includes +3% for Paypal)</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -660,6 +660,9 @@
       <c r="B3" s="2">
         <v>3</v>
       </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
@@ -715,7 +718,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
@@ -724,11 +727,14 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
+      <c r="C7" s="2">
+        <v>1.5</v>
+      </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -736,7 +742,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -814,7 +820,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B20" s="8">
         <f>SUM(B3:B19)</f>
@@ -824,8 +830,8 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10">
-        <f>SUM(F2:F19)</f>
-        <v>885</v>
+        <f>SUM(F2:F19)+3/100*(SUM(F2:F19))</f>
+        <v>911.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use Restify and POSTMAN to send HTTP POST request that generates the YAML file. OK. With tests.
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Task name</t>
   </si>
@@ -173,12 +173,30 @@
   <si>
     <t>Total: (Includes +3% for Paypal)</t>
   </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>Use Restify node client to receive POST requests and generate YAML file vlan id, vlan name)</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Payments: (€)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,13 +220,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -257,10 +299,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,8 +336,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,10 +665,11 @@
     <col min="4" max="4" width="20.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="20.5703125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -632,8 +688,11 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -652,8 +711,11 @@
       <c r="F2" s="6">
         <v>450</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -673,8 +735,11 @@
         <f>B3*30</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="G3" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -691,8 +756,11 @@
         <f t="shared" ref="F4:F19" si="0">B4*30</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -706,8 +774,11 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -725,7 +796,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -739,8 +810,11 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -751,50 +825,68 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -824,14 +916,24 @@
       </c>
       <c r="B20" s="8">
         <f>SUM(B3:B19)</f>
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10">
         <f>SUM(F2:F19)+3/100*(SUM(F2:F19))</f>
-        <v>911.55</v>
+        <v>1004.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>194.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use mkdirp node module to create recursively all folders. Creates host_vars and group_vars folder and put the expected files in these two folders.
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -186,9 +186,6 @@
     <t>Test: Use Restify node client</t>
   </si>
   <si>
-    <t>3h for the moment</t>
-  </si>
-  <si>
     <t>Use Promises</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Restify API for hsrp, ospf, svi</t>
+  </si>
+  <si>
+    <t>4h for the moment</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -800,7 +800,7 @@
         <v>45</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -839,13 +839,13 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Using handler in yamlWriter.
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Task name</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Restify API for hsrp, ospf, svi</t>
-  </si>
-  <si>
-    <t>4h40 for the moment</t>
   </si>
   <si>
     <t>Create folders dynamically</t>
@@ -686,7 +683,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +791,7 @@
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2">
         <v>0.5</v>
@@ -806,7 +803,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
@@ -878,8 +875,8 @@
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
+      <c r="C9" s="2">
+        <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>

</xml_diff>